<commit_message>
update sql sentences after that add company
</commit_message>
<xml_diff>
--- a/tecun-security-api/queries/SQL Sentences in Oracle.xlsx
+++ b/tecun-security-api/queries/SQL Sentences in Oracle.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santosj.MIXCO\repository\SSO_security\tecun-security\queries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santosj.MIXCO\repository\SSO_security\tecun-security-api\queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="111">
   <si>
     <t>rol_id</t>
   </si>
@@ -251,6 +251,114 @@
   </si>
   <si>
     <t>insert_drive_file</t>
+  </si>
+  <si>
+    <t>Paises</t>
+  </si>
+  <si>
+    <t>Ciudaddes</t>
+  </si>
+  <si>
+    <t>Tipo de barriles</t>
+  </si>
+  <si>
+    <t>Tipas o tanques</t>
+  </si>
+  <si>
+    <t>Tipos de tarimas</t>
+  </si>
+  <si>
+    <t>Tipos De incidencias</t>
+  </si>
+  <si>
+    <t>Tipos de maridajes</t>
+  </si>
+  <si>
+    <t>Motivos de incidencias</t>
+  </si>
+  <si>
+    <t>Empresas</t>
+  </si>
+  <si>
+    <t>Proveedores</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Bodegas</t>
+  </si>
+  <si>
+    <t>Piezas</t>
+  </si>
+  <si>
+    <t>Correlativos de procesos</t>
+  </si>
+  <si>
+    <t>Tipos de reparaciones</t>
+  </si>
+  <si>
+    <t>Motivos de baja</t>
+  </si>
+  <si>
+    <t>Motivo de traslado</t>
+  </si>
+  <si>
+    <t>/company</t>
+  </si>
+  <si>
+    <t>/country</t>
+  </si>
+  <si>
+    <t>/city</t>
+  </si>
+  <si>
+    <t>/barrelType</t>
+  </si>
+  <si>
+    <t>/pipe</t>
+  </si>
+  <si>
+    <t>/pallet</t>
+  </si>
+  <si>
+    <t>/incidentType</t>
+  </si>
+  <si>
+    <t>/pairingType</t>
+  </si>
+  <si>
+    <t>/incidenceReason</t>
+  </si>
+  <si>
+    <t>/supplier</t>
+  </si>
+  <si>
+    <t>/product</t>
+  </si>
+  <si>
+    <t>/warehouse</t>
+  </si>
+  <si>
+    <t>/piece</t>
+  </si>
+  <si>
+    <t>/process</t>
+  </si>
+  <si>
+    <t>/fixType</t>
+  </si>
+  <si>
+    <t>/cancellationReason</t>
+  </si>
+  <si>
+    <t>/transferReason</t>
+  </si>
+  <si>
+    <t>view_list</t>
+  </si>
+  <si>
+    <t>apartment</t>
   </si>
 </sst>
 </file>
@@ -266,7 +374,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +399,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -304,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -314,6 +428,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +722,8 @@
     <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41.42578125" bestFit="1" customWidth="1"/>
@@ -684,28 +801,28 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="8">
         <v>1</v>
       </c>
       <c r="I2" t="s">
@@ -747,29 +864,29 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="8">
         <f>+B2+1</f>
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="8">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="8">
         <v>1</v>
       </c>
       <c r="I3" t="s">
@@ -789,7 +906,7 @@
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O16" si="0">+CONCATENATE("INSERT INTO form (",N3,") values(",A3,",'",C3,"',",D3,",'",E3,"',",F3,",'",G3,"',",H3,",",I3,",",J3,",",K3,",",L3,",'",M3,"');")</f>
+        <f t="shared" ref="O3:O17" si="0">+CONCATENATE("INSERT INTO form (",N3,") values(",A3,",'",C3,"',",D3,",'",E3,"',",F3,",'",G3,"',",H3,",",I3,",",J3,",",K3,",",L3,",'",M3,"');")</f>
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',2,'/profile',1,'person',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P3" t="s">
@@ -811,29 +928,29 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B4">
-        <f t="shared" ref="B4:B16" si="3">+B3+1</f>
+      <c r="B4" s="8">
+        <f t="shared" ref="B4:B35" si="3">+B3+1</f>
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="8">
         <v>1</v>
       </c>
       <c r="I4" t="s">
@@ -849,7 +966,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N16" si="4">+N3</f>
+        <f t="shared" ref="N4:N35" si="4">+N3</f>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O4" t="str">
@@ -875,29 +992,29 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="8">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="8">
         <v>1</v>
       </c>
       <c r="I5" t="s">
@@ -939,29 +1056,29 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="8">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="8">
         <v>1</v>
       </c>
       <c r="I6" t="s">
@@ -1003,29 +1120,29 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="8">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="8">
         <v>1</v>
       </c>
       <c r="I7" t="s">
@@ -1067,29 +1184,29 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="8">
         <v>1</v>
       </c>
       <c r="I8" t="s">
@@ -1131,29 +1248,29 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="8">
         <v>1</v>
       </c>
       <c r="I9" t="s">
@@ -1195,29 +1312,29 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="8">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
         <v>2</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="8">
         <v>1</v>
       </c>
       <c r="I10" t="s">
@@ -1259,29 +1376,29 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="8">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="8">
         <v>1</v>
       </c>
       <c r="I11" t="s">
@@ -1323,29 +1440,29 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="8">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
         <v>2</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F12" s="8">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="8">
         <v>1</v>
       </c>
       <c r="I12" t="s">
@@ -1387,30 +1504,30 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="8">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13">
+      <c r="C13" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="8">
         <v>2</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
       </c>
       <c r="I13" t="s">
         <v>13</v>
@@ -1423,23 +1540,20 @@
       </c>
       <c r="L13">
         <v>0</v>
-      </c>
-      <c r="M13" t="s">
-        <v>50</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',6,'/',1,'home',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Home');</v>
+        <f t="shared" ref="O13" si="6">+CONCATENATE("INSERT INTO form (",N13,") values(",A13,",'",C13,"',",D13,",'",E13,"',",F13,",'",G13,"',",H13,",",I13,",",J13,",",K13,",",L13,",'",M13,"');")</f>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Empresas',2,'/company',1,'apartment',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P13" t="s">
         <v>62</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" ref="Q13:Q16" si="6">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <f t="shared" ref="Q13" si="7">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B13,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
         <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R13">
@@ -1449,7 +1563,7 @@
         <v>64</v>
       </c>
       <c r="T13" t="str">
-        <f t="shared" ref="T13:T16" si="7">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+1,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+2,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+3,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+4,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+5,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+6,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <f t="shared" ref="T13" si="8">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+1,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+2,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+3,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+4,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+5,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B13-1)*6)+6,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
         <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,67,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,68,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,69,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,70,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,71,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,72,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
@@ -1458,23 +1572,23 @@
         <v>60</v>
       </c>
       <c r="B14">
-        <f t="shared" si="3"/>
-        <v>13</v>
+        <f>+B12+1</f>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -1492,22 +1606,22 @@
         <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="4"/>
+        <f>+N12</f>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',7,'/profile',1,'person',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Profile');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',6,'/',1,'home',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Home');</v>
       </c>
       <c r="P14" t="s">
         <v>62</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" ref="Q14:Q17" si="9">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B14,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B14,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B14,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B14,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B14,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B14,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R14">
         <v>1</v>
@@ -1516,8 +1630,8 @@
         <v>64</v>
       </c>
       <c r="T14" t="str">
-        <f t="shared" si="7"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,73,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,74,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,75,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,76,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,77,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,78,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" ref="T14:T17" si="10">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B14-1)*6)+1,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B14-1)*6)+2,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B14-1)*6)+3,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B14-1)*6)+4,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B14-1)*6)+5,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B14-1)*6)+6,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,67,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,68,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,69,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,70,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,71,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,72,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1526,22 +1640,22 @@
       </c>
       <c r="B15">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -1559,7 +1673,7 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="4"/>
@@ -1567,14 +1681,14 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',8,'/barril',1,'battery-full',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Barrel');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',7,'/profile',1,'person',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Profile');</v>
       </c>
       <c r="P15" t="s">
         <v>62</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="9"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R15">
         <v>1</v>
@@ -1583,8 +1697,8 @@
         <v>64</v>
       </c>
       <c r="T15" t="str">
-        <f t="shared" si="7"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,79,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,80,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,81,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,82,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,83,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,84,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" si="10"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,73,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,74,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,75,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,76,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,77,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,78,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1593,22 +1707,22 @@
       </c>
       <c r="B16">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -1626,7 +1740,7 @@
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="4"/>
@@ -1634,14 +1748,14 @@
       </c>
       <c r="O16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',9,'/tarima',1,'dns',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Pallet');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',8,'/barril',1,'battery-full',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Barrel');</v>
       </c>
       <c r="P16" t="s">
         <v>62</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="9"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R16">
         <v>1</v>
@@ -1650,15 +1764,1231 @@
         <v>64</v>
       </c>
       <c r="T16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,79,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,80,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,81,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,82,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,83,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,84,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>53</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',9,'/tarima',1,'dns',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Pallet');</v>
+      </c>
+      <c r="P17" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17" t="s">
+        <v>64</v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" si="10"/>
         <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,85,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,86,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,87,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,88,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,89,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,90,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
-    <row r="20" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q20">
-        <f>((B6-1)*6)+5</f>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="8">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="8">
+        <v>11</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="8">
+        <v>3</v>
+      </c>
+      <c r="I18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" ref="O18:O35" si="11">+CONCATENATE("INSERT INTO form (",N18,") values(",A18,",'",C18,"',",D18,",'",E18,"',",F18,",'",G18,"',",H18,",",I18,",",J18,",",K18,",",L18,",'",M18,"');")</f>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',11,'/',1,'home',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P18" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" ref="Q18:Q35" si="12">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P18,",",B18,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P18,",",B18,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P18,",",B18,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P18,",",B18,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P18,",",B18,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P18,",",B18,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18" t="s">
+        <v>64</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" ref="T18:T35" si="13">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S18,",",((B18-1)*6)+1,",",R18,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S18,",",((B18-1)*6)+2,",",R18,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S18,",",((B18-1)*6)+3,",",R18,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S18,",",((B18-1)*6)+4,",",R18,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S18,",",((B18-1)*6)+5,",",R18,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S18,",",((B18-1)*6)+6,",",R18,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,91,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,92,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,93,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,94,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,95,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,96,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="8">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="8">
+        <v>12</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="8">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="11"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',12,'/profile',1,'person',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P19" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19" t="s">
+        <v>64</v>
+      </c>
+      <c r="T19" t="str">
+        <f t="shared" si="13"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,97,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,98,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,99,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,100,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,101,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,102,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="8">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="8">
+        <v>13</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="8">
+        <v>1</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="8">
+        <v>3</v>
+      </c>
+      <c r="I20" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" ref="O20:O35" si="14">+CONCATENATE("INSERT INTO form (",N20,") values(",A20,",'",C20,"',",D20,",'",E20,"',",F20,",'",G20,"',",H20,",",I20,",",J20,",",K20,",",L20,",'",M20,"');")</f>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Paises',13,'/country',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P20" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" ref="Q20:Q35" si="15">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P20,",",B20,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P20,",",B20,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P20,",",B20,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P20,",",B20,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P20,",",B20,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P20,",",B20,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,18,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,18,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,18,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,18,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,18,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,18,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20" t="s">
+        <v>64</v>
+      </c>
+      <c r="T20" t="str">
+        <f t="shared" ref="T20:T35" si="16">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S20,",",((B20-1)*6)+1,",",R20,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S20,",",((B20-1)*6)+2,",",R20,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S20,",",((B20-1)*6)+3,",",R20,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S20,",",((B20-1)*6)+4,",",R20,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S20,",",((B20-1)*6)+5,",",R20,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S20,",",((B20-1)*6)+6,",",R20,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,103,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,104,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,105,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,106,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,107,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,108,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="8">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="8">
+        <v>13</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="8">
+        <v>3</v>
+      </c>
+      <c r="I21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Ciudaddes',13,'/city',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,19,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,19,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,19,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,19,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,19,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,19,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21" t="s">
+        <v>64</v>
+      </c>
+      <c r="T21" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,109,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,110,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,111,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,112,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,113,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,114,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="8">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="8">
+        <v>13</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="8">
+        <v>1</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="8">
+        <v>3</v>
+      </c>
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tipo de barriles',13,'/barrelType',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P22" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,20,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,20,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,20,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,20,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,20,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,20,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22" t="s">
+        <v>64</v>
+      </c>
+      <c r="T22" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,115,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,116,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,117,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,118,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,119,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,120,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="8">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="8">
+        <v>13</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="8">
+        <v>3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" t="s">
+        <v>46</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tipas o tanques',13,'/pipe',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P23" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,21,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,21,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,21,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,21,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,21,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,21,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23" t="s">
+        <v>64</v>
+      </c>
+      <c r="T23" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,121,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,122,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,123,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,124,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,125,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,126,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="8">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="8">
+        <v>13</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="8">
+        <v>1</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="8">
+        <v>3</v>
+      </c>
+      <c r="I24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" t="s">
+        <v>46</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tipos de tarimas',13,'/pallet',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P24" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,22,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,22,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,22,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,22,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,22,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,22,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24" t="s">
+        <v>64</v>
+      </c>
+      <c r="T24" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,127,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,128,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,129,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,130,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,131,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,132,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="8">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="8">
+        <v>13</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="8">
+        <v>1</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H25" s="8">
+        <v>3</v>
+      </c>
+      <c r="I25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tipos De incidencias',13,'/incidentType',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P25" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,23,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,23,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,23,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,23,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,23,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,23,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25" t="s">
+        <v>64</v>
+      </c>
+      <c r="T25" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,133,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,134,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,135,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,136,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,137,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,138,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="8">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="8">
+        <v>13</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="8">
+        <v>1</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" s="8">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tipos de maridajes',13,'/pairingType',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P26" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q26" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,24,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,24,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,24,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,24,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,24,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,24,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26" t="s">
+        <v>64</v>
+      </c>
+      <c r="T26" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,139,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,140,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,141,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,142,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,143,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,144,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="8">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="8">
+        <v>13</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" s="8">
+        <v>1</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" s="8">
+        <v>3</v>
+      </c>
+      <c r="I27" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" t="s">
+        <v>46</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Motivos de incidencias',13,'/incidenceReason',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P27" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q27" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,25,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,25,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,25,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,25,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,25,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,25,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27" t="s">
+        <v>64</v>
+      </c>
+      <c r="T27" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,145,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,146,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,147,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,148,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,149,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,150,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="8">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="8">
+        <v>13</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" s="8">
+        <v>1</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="8">
+        <v>3</v>
+      </c>
+      <c r="I28" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" t="s">
+        <v>46</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Proveedores',13,'/supplier',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P28" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q28" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,26,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,26,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,26,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,26,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,26,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,26,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28" t="s">
+        <v>64</v>
+      </c>
+      <c r="T28" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,151,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,152,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,153,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,154,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,155,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,156,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="8">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="8">
+        <v>13</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="8">
+        <v>1</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H29" s="8">
+        <v>3</v>
+      </c>
+      <c r="I29" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" t="s">
+        <v>46</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Productos',13,'/product',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P29" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,27,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,27,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,27,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,27,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,27,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,27,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29" t="s">
+        <v>64</v>
+      </c>
+      <c r="T29" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,157,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,158,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,159,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,160,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,161,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,162,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="8">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="8">
+        <v>13</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" s="8">
+        <v>1</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="8">
+        <v>3</v>
+      </c>
+      <c r="I30" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Bodegas',13,'/warehouse',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P30" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,28,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,28,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,28,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,28,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,28,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,28,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30" t="s">
+        <v>64</v>
+      </c>
+      <c r="T30" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,163,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,164,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,165,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,166,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,167,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,168,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="8">
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
+      <c r="C31" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="8">
+        <v>13</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="8">
+        <v>1</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H31" s="8">
+        <v>3</v>
+      </c>
+      <c r="I31" t="s">
+        <v>13</v>
+      </c>
+      <c r="J31" t="s">
+        <v>46</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Piezas',13,'/piece',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P31" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,29,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,29,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,29,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,29,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,29,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,29,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31" t="s">
+        <v>64</v>
+      </c>
+      <c r="T31" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,169,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,170,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,171,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,172,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,173,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,174,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="8">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="8">
+        <v>13</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="8">
+        <v>1</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H32" s="8">
+        <v>3</v>
+      </c>
+      <c r="I32" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" t="s">
+        <v>46</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Correlativos de procesos',13,'/process',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P32" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,30,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,30,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,30,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,30,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,30,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,30,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32" t="s">
+        <v>64</v>
+      </c>
+      <c r="T32" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,175,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,176,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,177,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,178,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,179,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,180,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="8">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="8">
+        <v>13</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" s="8">
+        <v>1</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H33" s="8">
+        <v>3</v>
+      </c>
+      <c r="I33" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tipos de reparaciones',13,'/fixType',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P33" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,31,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,31,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,31,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,31,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,31,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,31,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33" t="s">
+        <v>64</v>
+      </c>
+      <c r="T33" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,181,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,182,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,183,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,184,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,185,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,186,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="8">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34" s="8">
+        <v>13</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="8">
+        <v>1</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H34" s="8">
+        <v>3</v>
+      </c>
+      <c r="I34" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" t="s">
+        <v>46</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Motivos de baja',13,'/cancellationReason',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P34" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,32,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,32,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,32,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,32,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,32,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,32,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R34">
+        <v>1</v>
+      </c>
+      <c r="S34" t="s">
+        <v>64</v>
+      </c>
+      <c r="T34" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,187,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,188,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,189,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,190,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,191,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,192,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="8">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="8">
+        <v>13</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="8">
+        <v>1</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H35" s="8">
+        <v>3</v>
+      </c>
+      <c r="I35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" t="s">
+        <v>46</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Motivo de traslado',13,'/transferReason',1,'view_list',3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P35" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,33,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,33,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,33,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,33,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,33,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,33,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R35">
+        <v>1</v>
+      </c>
+      <c r="S35" t="s">
+        <v>64</v>
+      </c>
+      <c r="T35" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,193,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,194,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,195,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,196,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,197,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,198,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
     </row>
   </sheetData>
   <sortState ref="B2:M14">

</xml_diff>